<commit_message>
💡 Mejoras al manual de usuario y estilos con Bootstrap
</commit_message>
<xml_diff>
--- a/incoming/Numero de facturas_1.xlsx
+++ b/incoming/Numero de facturas_1.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -506,10 +507,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2099992</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2099474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2097753</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1170</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,101 +704,7 @@
         <v>2100681</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2099992</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2099474</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2097753</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1170</v>
-      </c>
-      <c r="B23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1187</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>